<commit_message>
Updated Spanish for intake
</commit_message>
<xml_diff>
--- a/docassemble/MAEvictionDefense/data/sources/eviction_es.xlsx
+++ b/docassemble/MAEvictionDefense/data/sources/eviction_es.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5806" uniqueCount="2394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5734" uniqueCount="2394">
   <si>
     <t>interview</t>
   </si>
@@ -26223,7 +26223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H819"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A753" workbookViewId="0">
       <selection activeCell="I188" sqref="I188"/>
     </sheetView>
   </sheetViews>

</xml_diff>